<commit_message>
fixed datetime to date
</commit_message>
<xml_diff>
--- a/Accrued Interest.xlsx
+++ b/Accrued Interest.xlsx
@@ -573,7 +573,7 @@
         <v>60000</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6501358695652174</v>
+        <v>0.6463994565217391</v>
       </c>
     </row>
     <row r="5">
@@ -601,7 +601,7 @@
         <v>60000</v>
       </c>
       <c r="H5" t="n">
-        <v>1.950407608695652</v>
+        <v>1.939198369565217</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +629,7 @@
         <v>60000</v>
       </c>
       <c r="H6" t="n">
-        <v>1.182065217391304</v>
+        <v>1.175271739130435</v>
       </c>
     </row>
     <row r="7">
@@ -825,7 +825,7 @@
         <v>60000</v>
       </c>
       <c r="H13" t="n">
-        <v>0.6480978260869565</v>
+        <v>0.6440217391304348</v>
       </c>
     </row>
     <row r="14">
@@ -853,7 +853,7 @@
         <v>5600</v>
       </c>
       <c r="H14" t="n">
-        <v>3.294497282608695</v>
+        <v>3.273777173913043</v>
       </c>
     </row>
     <row r="15">
@@ -909,7 +909,7 @@
         <v>40000</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8641304347826086</v>
+        <v>0.8586956521739131</v>
       </c>
     </row>
     <row r="17">
@@ -1049,7 +1049,7 @@
         <v>60000</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4444060773480663</v>
+        <v>0.4412983425414365</v>
       </c>
     </row>
     <row r="22">
@@ -1077,7 +1077,7 @@
         <v>60000</v>
       </c>
       <c r="H22" t="n">
-        <v>1.827002762430939</v>
+        <v>1.814226519337017</v>
       </c>
     </row>
     <row r="23">
@@ -1105,7 +1105,7 @@
         <v>40000</v>
       </c>
       <c r="H23" t="n">
-        <v>1.086325966850829</v>
+        <v>1.078729281767956</v>
       </c>
     </row>
     <row r="24">
@@ -1245,7 +1245,7 @@
         <v>60000</v>
       </c>
       <c r="H28" t="n">
-        <v>0.6187845303867403</v>
+        <v>0.613950276243094</v>
       </c>
     </row>
     <row r="29">
@@ -1357,7 +1357,7 @@
         <v>60000</v>
       </c>
       <c r="H32" t="n">
-        <v>1.202953296703297</v>
+        <v>1.192307692307692</v>
       </c>
     </row>
     <row r="33">
@@ -1385,7 +1385,7 @@
         <v>40000</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1552197802197802</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="34">
@@ -1413,7 +1413,7 @@
         <v>10000</v>
       </c>
       <c r="H34" t="n">
-        <v>0.8149038461538461</v>
+        <v>0.8076923076923077</v>
       </c>
     </row>
     <row r="35">
@@ -1581,7 +1581,7 @@
         <v>10000</v>
       </c>
       <c r="H40" t="n">
-        <v>0.7067307692307692</v>
+        <v>0.6995192307692307</v>
       </c>
     </row>
     <row r="41">
@@ -1721,7 +1721,7 @@
         <v>60000</v>
       </c>
       <c r="H45" t="n">
-        <v>0.8777624309392266</v>
+        <v>0.8670580110497238</v>
       </c>
     </row>
     <row r="46">
@@ -1749,7 +1749,7 @@
         <v>60000</v>
       </c>
       <c r="H46" t="n">
-        <v>0.08494475138121547</v>
+        <v>0.08390883977900553</v>
       </c>
     </row>
     <row r="47">
@@ -1777,7 +1777,7 @@
         <v>10000</v>
       </c>
       <c r="H47" t="n">
-        <v>0.6512430939226519</v>
+        <v>0.6433011049723757</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>60000</v>
       </c>
       <c r="H54" t="n">
-        <v>0.3933011049723757</v>
+        <v>0.3874309392265193</v>
       </c>
     </row>
     <row r="55">
@@ -2029,7 +2029,7 @@
         <v>60000</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5089779005524862</v>
+        <v>0.5013812154696132</v>
       </c>
     </row>
     <row r="57">
@@ -2141,7 +2141,7 @@
         <v>10000</v>
       </c>
       <c r="H60" t="n">
-        <v>0.6071428571428571</v>
+        <v>0.595467032967033</v>
       </c>
     </row>
     <row r="61">
@@ -2169,7 +2169,7 @@
         <v>60000</v>
       </c>
       <c r="H61" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.03502747252747253</v>
       </c>
     </row>
     <row r="62">
@@ -2197,7 +2197,7 @@
         <v>10000</v>
       </c>
       <c r="H62" t="n">
-        <v>0.4107142857142857</v>
+        <v>0.4028159340659341</v>
       </c>
     </row>
     <row r="63">
@@ -2281,7 +2281,7 @@
         <v>10000</v>
       </c>
       <c r="H65" t="n">
-        <v>0.292239010989011</v>
+        <v>0.2843406593406593</v>
       </c>
     </row>
     <row r="66">
@@ -2365,7 +2365,7 @@
         <v>40000</v>
       </c>
       <c r="H68" t="n">
-        <v>0.2683011049723757</v>
+        <v>0.255524861878453</v>
       </c>
     </row>
     <row r="69">
@@ -2393,7 +2393,7 @@
         <v>10000</v>
       </c>
       <c r="H69" t="n">
-        <v>0.01450276243093923</v>
+        <v>0.0138121546961326</v>
       </c>
     </row>
     <row r="70">
@@ -2421,7 +2421,7 @@
         <v>10000</v>
       </c>
       <c r="H70" t="n">
-        <v>0.1595303867403315</v>
+        <v>0.1519337016574586</v>
       </c>
     </row>
     <row r="71">
@@ -2505,7 +2505,7 @@
         <v>60000</v>
       </c>
       <c r="H73" t="n">
-        <v>0.04972375690607735</v>
+        <v>0.04143646408839779</v>
       </c>
     </row>
     <row r="74">
@@ -2561,7 +2561,7 @@
         <v>10000</v>
       </c>
       <c r="H75" t="n">
-        <v>0.1182065217391304</v>
+        <v>0.1175271739130435</v>
       </c>
     </row>
     <row r="76">
@@ -2589,7 +2589,7 @@
         <v>60000</v>
       </c>
       <c r="H76" t="n">
-        <v>2.245923913043478</v>
+        <v>2.233016304347826</v>
       </c>
     </row>
     <row r="77">
@@ -2617,7 +2617,7 @@
         <v>10000</v>
       </c>
       <c r="H77" t="n">
-        <v>1.359375</v>
+        <v>1.3515625</v>
       </c>
     </row>
     <row r="78">
@@ -2729,7 +2729,7 @@
         <v>35000</v>
       </c>
       <c r="H81" t="n">
-        <v>1.350203804347826</v>
+        <v>1.341711956521739</v>
       </c>
     </row>
     <row r="82">
@@ -2785,7 +2785,7 @@
         <v>5600</v>
       </c>
       <c r="H83" t="n">
-        <v>0.8641304347826086</v>
+        <v>0.8586956521739131</v>
       </c>
     </row>
     <row r="84">
@@ -2813,7 +2813,7 @@
         <v>5000</v>
       </c>
       <c r="H84" t="n">
-        <v>2.970448369565217</v>
+        <v>2.951766304347826</v>
       </c>
     </row>
     <row r="85">
@@ -2841,7 +2841,7 @@
         <v>60000</v>
       </c>
       <c r="H85" t="n">
-        <v>0.09875690607734806</v>
+        <v>0.09806629834254144</v>
       </c>
     </row>
     <row r="86">
@@ -2869,7 +2869,7 @@
         <v>60000</v>
       </c>
       <c r="H86" t="n">
-        <v>1.975138121546961</v>
+        <v>1.961325966850829</v>
       </c>
     </row>
     <row r="87">
@@ -2897,7 +2897,7 @@
         <v>60000</v>
       </c>
       <c r="H87" t="n">
-        <v>1.086325966850829</v>
+        <v>1.078729281767956</v>
       </c>
     </row>
     <row r="88">
@@ -2953,7 +2953,7 @@
         <v>10000</v>
       </c>
       <c r="H89" t="n">
-        <v>1.237569060773481</v>
+        <v>1.227900552486188</v>
       </c>
     </row>
     <row r="90">
@@ -2981,7 +2981,7 @@
         <v>10000</v>
       </c>
       <c r="H90" t="n">
-        <v>1.552197802197802</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="91">
@@ -3009,7 +3009,7 @@
         <v>40000</v>
       </c>
       <c r="H91" t="n">
-        <v>0.07760989010989011</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="92">
@@ -3037,7 +3037,7 @@
         <v>5600</v>
       </c>
       <c r="H92" t="n">
-        <v>0.9313186813186813</v>
+        <v>0.9230769230769231</v>
       </c>
     </row>
     <row r="93">
@@ -3093,7 +3093,7 @@
         <v>5600</v>
       </c>
       <c r="H94" t="n">
-        <v>1.144230769230769</v>
+        <v>1.132554945054945</v>
       </c>
     </row>
     <row r="95">
@@ -3149,7 +3149,7 @@
         <v>8000</v>
       </c>
       <c r="H96" t="n">
-        <v>0.05662983425414365</v>
+        <v>0.05593922651933702</v>
       </c>
     </row>
     <row r="97">
@@ -3177,7 +3177,7 @@
         <v>10000</v>
       </c>
       <c r="H97" t="n">
-        <v>1.132596685082873</v>
+        <v>1.11878453038674</v>
       </c>
     </row>
     <row r="98">
@@ -3205,7 +3205,7 @@
         <v>40000</v>
       </c>
       <c r="H98" t="n">
-        <v>0.6795580110497238</v>
+        <v>0.6712707182320442</v>
       </c>
     </row>
     <row r="99">
@@ -3233,7 +3233,7 @@
         <v>50000</v>
       </c>
       <c r="H99" t="n">
-        <v>0.4164364640883978</v>
+        <v>0.4102209944751381</v>
       </c>
     </row>
     <row r="100">
@@ -3289,7 +3289,7 @@
         <v>40000</v>
       </c>
       <c r="H101" t="n">
-        <v>0.8328729281767956</v>
+        <v>0.8204419889502762</v>
       </c>
     </row>
     <row r="102">
@@ -3373,7 +3373,7 @@
         <v>50000</v>
       </c>
       <c r="H104" t="n">
-        <v>0.05357142857142857</v>
+        <v>0.05254120879120879</v>
       </c>
     </row>
     <row r="105">
@@ -3401,7 +3401,7 @@
         <v>40000</v>
       </c>
       <c r="H105" t="n">
-        <v>0.6964285714285714</v>
+        <v>0.6830357142857143</v>
       </c>
     </row>
     <row r="106">
@@ -3429,7 +3429,7 @@
         <v>40000</v>
       </c>
       <c r="H106" t="n">
-        <v>0.4107142857142857</v>
+        <v>0.4028159340659341</v>
       </c>
     </row>
     <row r="107">
@@ -3457,7 +3457,7 @@
         <v>40000</v>
       </c>
       <c r="H107" t="n">
-        <v>0.4065934065934066</v>
+        <v>0.3956043956043956</v>
       </c>
     </row>
     <row r="108">
@@ -3513,7 +3513,7 @@
         <v>40000</v>
       </c>
       <c r="H109" t="n">
-        <v>0.2465469613259668</v>
+        <v>0.2348066298342542</v>
       </c>
     </row>
     <row r="110">
@@ -3541,7 +3541,7 @@
         <v>40000</v>
       </c>
       <c r="H110" t="n">
-        <v>0.1522790055248619</v>
+        <v>0.1450276243093923</v>
       </c>
     </row>
     <row r="111">
@@ -3569,7 +3569,7 @@
         <v>50000</v>
       </c>
       <c r="H111" t="n">
-        <v>0.02175414364640884</v>
+        <v>0.02071823204419889</v>
       </c>
     </row>
     <row r="112">
@@ -3597,7 +3597,7 @@
         <v>40000</v>
       </c>
       <c r="H112" t="n">
-        <v>0.06422651933701658</v>
+        <v>0.05352209944751381</v>
       </c>
     </row>
     <row r="113">
@@ -3625,7 +3625,7 @@
         <v>50000</v>
       </c>
       <c r="H113" t="n">
-        <v>2.009510869565217</v>
+        <v>1.997961956521739</v>
       </c>
     </row>
     <row r="114">
@@ -3653,7 +3653,7 @@
         <v>50000</v>
       </c>
       <c r="H114" t="n">
-        <v>1.24116847826087</v>
+        <v>1.234035326086957</v>
       </c>
     </row>
     <row r="115">
@@ -3681,7 +3681,7 @@
         <v>50000</v>
       </c>
       <c r="H115" t="n">
-        <v>0.1773097826086956</v>
+        <v>0.1762907608695652</v>
       </c>
     </row>
     <row r="116">
@@ -3737,7 +3737,7 @@
         <v>10000</v>
       </c>
       <c r="H117" t="n">
-        <v>1.728260869565217</v>
+        <v>1.717391304347826</v>
       </c>
     </row>
     <row r="118">
@@ -3765,7 +3765,7 @@
         <v>5000</v>
       </c>
       <c r="H118" t="n">
-        <v>2.592391304347826</v>
+        <v>2.576086956521739</v>
       </c>
     </row>
     <row r="119">
@@ -3821,7 +3821,7 @@
         <v>28000</v>
       </c>
       <c r="H120" t="n">
-        <v>0.7021059782608695</v>
+        <v>0.6976902173913043</v>
       </c>
     </row>
     <row r="121">
@@ -3849,7 +3849,7 @@
         <v>50000</v>
       </c>
       <c r="H121" t="n">
-        <v>1.827002762430939</v>
+        <v>1.814226519337017</v>
       </c>
     </row>
     <row r="122">
@@ -3877,7 +3877,7 @@
         <v>19000</v>
       </c>
       <c r="H122" t="n">
-        <v>0.9875690607734806</v>
+        <v>0.9806629834254144</v>
       </c>
     </row>
     <row r="123">
@@ -3905,7 +3905,7 @@
         <v>40000</v>
       </c>
       <c r="H123" t="n">
-        <v>0.1975138121546961</v>
+        <v>0.1961325966850829</v>
       </c>
     </row>
     <row r="124">
@@ -3933,7 +3933,7 @@
         <v>40000</v>
       </c>
       <c r="H124" t="n">
-        <v>1.635359116022099</v>
+        <v>1.622582872928177</v>
       </c>
     </row>
     <row r="125">
@@ -3961,7 +3961,7 @@
         <v>50000</v>
       </c>
       <c r="H125" t="n">
-        <v>0.6984890109890109</v>
+        <v>0.6923076923076923</v>
       </c>
     </row>
     <row r="126">
@@ -3989,7 +3989,7 @@
         <v>40000</v>
       </c>
       <c r="H126" t="n">
-        <v>0.2328296703296703</v>
+        <v>0.2307692307692308</v>
       </c>
     </row>
     <row r="127">
@@ -4017,7 +4017,7 @@
         <v>40000</v>
       </c>
       <c r="H127" t="n">
-        <v>1.396978021978022</v>
+        <v>1.384615384615385</v>
       </c>
     </row>
     <row r="128">
@@ -4045,7 +4045,7 @@
         <v>50000</v>
       </c>
       <c r="H128" t="n">
-        <v>1.009615384615385</v>
+        <v>0.9993131868131868</v>
       </c>
     </row>
     <row r="129">
@@ -4073,7 +4073,7 @@
         <v>40000</v>
       </c>
       <c r="H129" t="n">
-        <v>0.1698895027624309</v>
+        <v>0.1678176795580111</v>
       </c>
     </row>
     <row r="130">
@@ -4101,7 +4101,7 @@
         <v>10000</v>
       </c>
       <c r="H130" t="n">
-        <v>0.5379834254143646</v>
+        <v>0.5314226519337016</v>
       </c>
     </row>
     <row r="131">
@@ -4129,7 +4129,7 @@
         <v>5000</v>
       </c>
       <c r="H131" t="n">
-        <v>1.104281767955801</v>
+        <v>1.090814917127072</v>
       </c>
     </row>
     <row r="132">
@@ -4157,7 +4157,7 @@
         <v>40000</v>
       </c>
       <c r="H132" t="n">
-        <v>0.6709254143646409</v>
+        <v>0.6609116022099447</v>
       </c>
     </row>
     <row r="133">
@@ -4241,7 +4241,7 @@
         <v>8000</v>
       </c>
       <c r="H135" t="n">
-        <v>0.3007596685082873</v>
+        <v>0.2962707182320442</v>
       </c>
     </row>
     <row r="136">
@@ -4269,7 +4269,7 @@
         <v>40000</v>
       </c>
       <c r="H136" t="n">
-        <v>0.3035714285714285</v>
+        <v>0.2977335164835165</v>
       </c>
     </row>
     <row r="137">
@@ -4297,7 +4297,7 @@
         <v>80000</v>
       </c>
       <c r="H137" t="n">
-        <v>0.6964285714285714</v>
+        <v>0.6830357142857143</v>
       </c>
     </row>
     <row r="138">
@@ -4325,7 +4325,7 @@
         <v>40000</v>
       </c>
       <c r="H138" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.1050824175824176</v>
       </c>
     </row>
     <row r="139">
@@ -4353,7 +4353,7 @@
         <v>80000</v>
       </c>
       <c r="H139" t="n">
-        <v>0.4192994505494506</v>
+        <v>0.407967032967033</v>
       </c>
     </row>
     <row r="140">
@@ -4381,7 +4381,7 @@
         <v>80000</v>
       </c>
       <c r="H140" t="n">
-        <v>0.2683011049723757</v>
+        <v>0.255524861878453</v>
       </c>
     </row>
     <row r="141">
@@ -4409,7 +4409,7 @@
         <v>80000</v>
       </c>
       <c r="H141" t="n">
-        <v>0.05075966850828729</v>
+        <v>0.04834254143646409</v>
       </c>
     </row>
     <row r="142">
@@ -4437,7 +4437,7 @@
         <v>2800</v>
       </c>
       <c r="H142" t="n">
-        <v>0.1087707182320442</v>
+        <v>0.1035911602209945</v>
       </c>
     </row>
     <row r="143">
@@ -4465,7 +4465,7 @@
         <v>40000</v>
       </c>
       <c r="H143" t="n">
-        <v>0.07458563535911603</v>
+        <v>0.06215469613259669</v>
       </c>
     </row>
     <row r="144">
@@ -4493,7 +4493,7 @@
         <v>40000</v>
       </c>
       <c r="H144" t="n">
-        <v>2.068614130434783</v>
+        <v>2.056725543478261</v>
       </c>
     </row>
     <row r="145">
@@ -4521,7 +4521,7 @@
         <v>40000</v>
       </c>
       <c r="H145" t="n">
-        <v>0.8865489130434783</v>
+        <v>0.8814538043478261</v>
       </c>
     </row>
     <row r="146">
@@ -4549,7 +4549,7 @@
         <v>40000</v>
       </c>
       <c r="H146" t="n">
-        <v>0.2955163043478261</v>
+        <v>0.2938179347826087</v>
       </c>
     </row>
     <row r="147">
@@ -4577,7 +4577,7 @@
         <v>40000</v>
       </c>
       <c r="H147" t="n">
-        <v>0.6480978260869565</v>
+        <v>0.6440217391304348</v>
       </c>
     </row>
     <row r="148">
@@ -4633,7 +4633,7 @@
         <v>40000</v>
       </c>
       <c r="H149" t="n">
-        <v>1.890285326086956</v>
+        <v>1.878396739130435</v>
       </c>
     </row>
     <row r="150">
@@ -4689,7 +4689,7 @@
         <v>2800</v>
       </c>
       <c r="H151" t="n">
-        <v>2.916440217391304</v>
+        <v>2.898097826086957</v>
       </c>
     </row>
     <row r="152">
@@ -4745,7 +4745,7 @@
         <v>40000</v>
       </c>
       <c r="H153" t="n">
-        <v>1.481353591160221</v>
+        <v>1.470994475138122</v>
       </c>
     </row>
     <row r="154">
@@ -4773,7 +4773,7 @@
         <v>70000</v>
       </c>
       <c r="H154" t="n">
-        <v>0.2962707182320442</v>
+        <v>0.2941988950276243</v>
       </c>
     </row>
     <row r="155">
@@ -4801,7 +4801,7 @@
         <v>40000</v>
       </c>
       <c r="H155" t="n">
-        <v>0.5431629834254144</v>
+        <v>0.539364640883978</v>
       </c>
     </row>
     <row r="156">
@@ -4829,7 +4829,7 @@
         <v>70000</v>
       </c>
       <c r="H156" t="n">
-        <v>1.635359116022099</v>
+        <v>1.622582872928177</v>
       </c>
     </row>
     <row r="157">
@@ -4857,7 +4857,7 @@
         <v>150000</v>
       </c>
       <c r="H157" t="n">
-        <v>1.086538461538462</v>
+        <v>1.076923076923077</v>
       </c>
     </row>
     <row r="158">
@@ -4885,7 +4885,7 @@
         <v>70000</v>
       </c>
       <c r="H158" t="n">
-        <v>0.2716346153846154</v>
+        <v>0.2692307692307692</v>
       </c>
     </row>
     <row r="159">
@@ -4913,7 +4913,7 @@
         <v>40000</v>
       </c>
       <c r="H159" t="n">
-        <v>0.5044642857142857</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="160">
@@ -4941,7 +4941,7 @@
         <v>70000</v>
       </c>
       <c r="H160" t="n">
-        <v>1.245192307692308</v>
+        <v>1.232486263736264</v>
       </c>
     </row>
     <row r="161">
@@ -4969,7 +4969,7 @@
         <v>40000</v>
       </c>
       <c r="H161" t="n">
-        <v>0.2548342541436464</v>
+        <v>0.2517265193370166</v>
       </c>
     </row>
     <row r="162">
@@ -4997,7 +4997,7 @@
         <v>10000</v>
       </c>
       <c r="H162" t="n">
-        <v>0.9343922651933702</v>
+        <v>0.9229972375690608</v>
       </c>
     </row>
     <row r="163">
@@ -5025,7 +5025,7 @@
         <v>40000</v>
       </c>
       <c r="H163" t="n">
-        <v>0.3680939226519337</v>
+        <v>0.3636049723756906</v>
       </c>
     </row>
     <row r="164">
@@ -5053,7 +5053,7 @@
         <v>2800</v>
       </c>
       <c r="H164" t="n">
-        <v>1.203038674033149</v>
+        <v>1.185082872928177</v>
       </c>
     </row>
     <row r="165">
@@ -5081,7 +5081,7 @@
         <v>70000</v>
       </c>
       <c r="H165" t="n">
-        <v>0.3701657458563536</v>
+        <v>0.3646408839779006</v>
       </c>
     </row>
     <row r="166">
@@ -5165,7 +5165,7 @@
         <v>10000</v>
       </c>
       <c r="H168" t="n">
-        <v>0.8560082872928176</v>
+        <v>0.8432320441988951</v>
       </c>
     </row>
     <row r="169">
@@ -5221,7 +5221,7 @@
         <v>70000</v>
       </c>
       <c r="H170" t="n">
-        <v>0.1785714285714285</v>
+        <v>0.1751373626373626</v>
       </c>
     </row>
     <row r="171">
@@ -5249,7 +5249,7 @@
         <v>70000</v>
       </c>
       <c r="H171" t="n">
-        <v>0.6071428571428571</v>
+        <v>0.595467032967033</v>
       </c>
     </row>
     <row r="172">
@@ -5277,7 +5277,7 @@
         <v>40000</v>
       </c>
       <c r="H172" t="n">
-        <v>0.2321428571428571</v>
+        <v>0.2276785714285714</v>
       </c>
     </row>
     <row r="173">
@@ -5305,7 +5305,7 @@
         <v>70000</v>
       </c>
       <c r="H173" t="n">
-        <v>0.4447115384615384</v>
+        <v>0.4326923076923077</v>
       </c>
     </row>
     <row r="174">
@@ -5333,7 +5333,7 @@
         <v>70000</v>
       </c>
       <c r="H174" t="n">
-        <v>0.07251381215469613</v>
+        <v>0.06906077348066299</v>
       </c>
     </row>
     <row r="175">
@@ -5361,7 +5361,7 @@
         <v>10000</v>
       </c>
       <c r="H175" t="n">
-        <v>0.1015193370165746</v>
+        <v>0.09668508287292818</v>
       </c>
     </row>
     <row r="176">
@@ -5389,7 +5389,7 @@
         <v>150000</v>
       </c>
       <c r="H176" t="n">
-        <v>0.2465469613259668</v>
+        <v>0.2348066298342542</v>
       </c>
     </row>
     <row r="177">
@@ -5417,7 +5417,7 @@
         <v>10000</v>
       </c>
       <c r="H177" t="n">
-        <v>0.06629834254143646</v>
+        <v>0.05524861878453038</v>
       </c>
     </row>
     <row r="178">
@@ -5445,7 +5445,7 @@
         <v>40000</v>
       </c>
       <c r="H178" t="n">
-        <v>0.7092391304347826</v>
+        <v>0.7051630434782609</v>
       </c>
     </row>
     <row r="179">
@@ -5473,7 +5473,7 @@
         <v>5000</v>
       </c>
       <c r="H179" t="n">
-        <v>2.862432065217391</v>
+        <v>2.844429347826087</v>
       </c>
     </row>
     <row r="180">
@@ -5585,7 +5585,7 @@
         <v>40000</v>
       </c>
       <c r="H183" t="n">
-        <v>0.9721467391304347</v>
+        <v>0.9660326086956522</v>
       </c>
     </row>
     <row r="184">
@@ -5613,7 +5613,7 @@
         <v>40000</v>
       </c>
       <c r="H184" t="n">
-        <v>1.78226902173913</v>
+        <v>1.771059782608696</v>
       </c>
     </row>
     <row r="185">
@@ -5641,7 +5641,7 @@
         <v>40000</v>
       </c>
       <c r="H185" t="n">
-        <v>0.4444060773480663</v>
+        <v>0.4412983425414365</v>
       </c>
     </row>
     <row r="186">
@@ -5669,7 +5669,7 @@
         <v>70000</v>
       </c>
       <c r="H186" t="n">
-        <v>0.7406767955801105</v>
+        <v>0.7354972375690608</v>
       </c>
     </row>
     <row r="187">
@@ -5697,7 +5697,7 @@
         <v>70000</v>
       </c>
       <c r="H187" t="n">
-        <v>1.502762430939226</v>
+        <v>1.491022099447514</v>
       </c>
     </row>
     <row r="188">
@@ -5725,7 +5725,7 @@
         <v>40000</v>
       </c>
       <c r="H188" t="n">
-        <v>0.1940247252747253</v>
+        <v>0.1923076923076923</v>
       </c>
     </row>
     <row r="189">
@@ -5753,7 +5753,7 @@
         <v>40000</v>
       </c>
       <c r="H189" t="n">
-        <v>0.7760989010989011</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="190">
@@ -5781,7 +5781,7 @@
         <v>40000</v>
       </c>
       <c r="H190" t="n">
-        <v>1.211538461538461</v>
+        <v>1.199175824175824</v>
       </c>
     </row>
     <row r="191">
@@ -5809,7 +5809,7 @@
         <v>70000</v>
       </c>
       <c r="H191" t="n">
-        <v>0.6229281767955801</v>
+        <v>0.6153314917127072</v>
       </c>
     </row>
     <row r="192">
@@ -5837,7 +5837,7 @@
         <v>70000</v>
       </c>
       <c r="H192" t="n">
-        <v>0.1132596685082873</v>
+        <v>0.111878453038674</v>
       </c>
     </row>
     <row r="193">
@@ -5865,7 +5865,7 @@
         <v>40000</v>
       </c>
       <c r="H193" t="n">
-        <v>0.8328729281767956</v>
+        <v>0.8204419889502762</v>
       </c>
     </row>
     <row r="194">
@@ -5921,7 +5921,7 @@
         <v>40000</v>
       </c>
       <c r="H195" t="n">
-        <v>0.4395718232044199</v>
+        <v>0.4330110497237569</v>
       </c>
     </row>
     <row r="196">
@@ -5977,7 +5977,7 @@
         <v>40000</v>
       </c>
       <c r="H197" t="n">
-        <v>0.375</v>
+        <v>0.3677884615384616</v>
       </c>
     </row>
     <row r="198">
@@ -6005,7 +6005,7 @@
         <v>40000</v>
       </c>
       <c r="H198" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.07005494505494506</v>
       </c>
     </row>
     <row r="199">
@@ -6033,7 +6033,7 @@
         <v>40000</v>
       </c>
       <c r="H199" t="n">
-        <v>0.4701236263736264</v>
+        <v>0.4574175824175824</v>
       </c>
     </row>
     <row r="200">
@@ -6061,7 +6061,7 @@
         <v>40000</v>
       </c>
       <c r="H200" t="n">
-        <v>0.1885359116022099</v>
+        <v>0.1795580110497238</v>
       </c>
     </row>
     <row r="201">
@@ -6089,7 +6089,7 @@
         <v>65000</v>
       </c>
       <c r="H201" t="n">
-        <v>0.02900552486187845</v>
+        <v>0.02762430939226519</v>
       </c>
     </row>
     <row r="202">
@@ -6117,7 +6117,7 @@
         <v>40000</v>
       </c>
       <c r="H202" t="n">
-        <v>0.07251381215469613</v>
+        <v>0.06042817679558011</v>
       </c>
     </row>
     <row r="203">
@@ -6145,7 +6145,7 @@
         <v>40000</v>
       </c>
       <c r="H203" t="n">
-        <v>0.1773097826086956</v>
+        <v>0.1762907608695652</v>
       </c>
     </row>
     <row r="204">
@@ -6173,7 +6173,7 @@
         <v>65000</v>
       </c>
       <c r="H204" t="n">
-        <v>1.300271739130435</v>
+        <v>1.292798913043478</v>
       </c>
     </row>
     <row r="205">
@@ -6229,7 +6229,7 @@
         <v>5000</v>
       </c>
       <c r="H206" t="n">
-        <v>1.620244565217391</v>
+        <v>1.610054347826087</v>
       </c>
     </row>
     <row r="207">
@@ -6285,7 +6285,7 @@
         <v>5000</v>
       </c>
       <c r="H208" t="n">
-        <v>2.754415760869565</v>
+        <v>2.737092391304348</v>
       </c>
     </row>
     <row r="209">
@@ -6313,7 +6313,7 @@
         <v>40000</v>
       </c>
       <c r="H209" t="n">
-        <v>0.9721467391304347</v>
+        <v>0.9660326086956522</v>
       </c>
     </row>
     <row r="210">
@@ -6341,7 +6341,7 @@
         <v>40000</v>
       </c>
       <c r="H210" t="n">
-        <v>0.1975138121546961</v>
+        <v>0.1961325966850829</v>
       </c>
     </row>
     <row r="211">
@@ -6369,7 +6369,7 @@
         <v>40000</v>
       </c>
       <c r="H211" t="n">
-        <v>1.234461325966851</v>
+        <v>1.225828729281768</v>
       </c>
     </row>
     <row r="212">
@@ -6397,7 +6397,7 @@
         <v>125000</v>
       </c>
       <c r="H212" t="n">
-        <v>1.193370165745856</v>
+        <v>1.184046961325967</v>
       </c>
     </row>
     <row r="213">
@@ -6425,7 +6425,7 @@
         <v>40000</v>
       </c>
       <c r="H213" t="n">
-        <v>1.280563186813187</v>
+        <v>1.269230769230769</v>
       </c>
     </row>
     <row r="214">
@@ -6453,7 +6453,7 @@
         <v>40000</v>
       </c>
       <c r="H214" t="n">
-        <v>0.1164148351648352</v>
+        <v>0.1153846153846154</v>
       </c>
     </row>
     <row r="215">
@@ -6481,7 +6481,7 @@
         <v>10000</v>
       </c>
       <c r="H215" t="n">
-        <v>1.043269230769231</v>
+        <v>1.032623626373626</v>
       </c>
     </row>
     <row r="216">
@@ -6509,7 +6509,7 @@
         <v>65000</v>
       </c>
       <c r="H216" t="n">
-        <v>0.9343922651933702</v>
+        <v>0.9229972375690608</v>
       </c>
     </row>
     <row r="217">
@@ -6537,7 +6537,7 @@
         <v>40000</v>
       </c>
       <c r="H217" t="n">
-        <v>0.1132596685082873</v>
+        <v>0.111878453038674</v>
       </c>
     </row>
     <row r="218">
@@ -6593,7 +6593,7 @@
         <v>2000</v>
       </c>
       <c r="H219" t="n">
-        <v>1.133632596685083</v>
+        <v>1.11671270718232</v>
       </c>
     </row>
     <row r="220">
@@ -6621,7 +6621,7 @@
         <v>40000</v>
       </c>
       <c r="H220" t="n">
-        <v>0.7634668508287292</v>
+        <v>0.7520718232044199</v>
       </c>
     </row>
     <row r="221">
@@ -6705,7 +6705,7 @@
         <v>40000</v>
       </c>
       <c r="H223" t="n">
-        <v>0.4164364640883978</v>
+        <v>0.4102209944751381</v>
       </c>
     </row>
     <row r="224">
@@ -6733,7 +6733,7 @@
         <v>40000</v>
       </c>
       <c r="H224" t="n">
-        <v>0.5535714285714285</v>
+        <v>0.5429258241758241</v>
       </c>
     </row>
     <row r="225">
@@ -6761,7 +6761,7 @@
         <v>40000</v>
       </c>
       <c r="H225" t="n">
-        <v>0.08928571428571427</v>
+        <v>0.08756868131868131</v>
       </c>
     </row>
     <row r="226">
@@ -6789,7 +6789,7 @@
         <v>125000</v>
       </c>
       <c r="H226" t="n">
-        <v>0.4065934065934066</v>
+        <v>0.3956043956043956</v>
       </c>
     </row>
     <row r="227">
@@ -6817,7 +6817,7 @@
         <v>40000</v>
       </c>
       <c r="H227" t="n">
-        <v>0.03625690607734806</v>
+        <v>0.03453038674033149</v>
       </c>
     </row>
     <row r="228">
@@ -6845,7 +6845,7 @@
         <v>40000</v>
       </c>
       <c r="H228" t="n">
-        <v>0.224792817679558</v>
+        <v>0.2140883977900553</v>
       </c>
     </row>
     <row r="229">
@@ -6873,7 +6873,7 @@
         <v>45000</v>
       </c>
       <c r="H229" t="n">
-        <v>0.07044198895027624</v>
+        <v>0.05870165745856354</v>
       </c>
     </row>
     <row r="230">
@@ -6901,7 +6901,7 @@
         <v>65000</v>
       </c>
       <c r="H230" t="n">
-        <v>1.654891304347826</v>
+        <v>1.645380434782609</v>
       </c>
     </row>
     <row r="231">
@@ -6929,7 +6929,7 @@
         <v>40000</v>
       </c>
       <c r="H231" t="n">
-        <v>0.3546195652173913</v>
+        <v>0.3525815217391304</v>
       </c>
     </row>
     <row r="232">
@@ -6985,7 +6985,7 @@
         <v>40000</v>
       </c>
       <c r="H233" t="n">
-        <v>1.188179347826087</v>
+        <v>1.18070652173913</v>
       </c>
     </row>
     <row r="234">
@@ -7041,7 +7041,7 @@
         <v>40000</v>
       </c>
       <c r="H235" t="n">
-        <v>1.580110497237569</v>
+        <v>1.569060773480663</v>
       </c>
     </row>
     <row r="236">
@@ -7069,7 +7069,7 @@
         <v>40000</v>
       </c>
       <c r="H236" t="n">
-        <v>0.4444060773480663</v>
+        <v>0.4412983425414365</v>
       </c>
     </row>
     <row r="237">
@@ -7097,7 +7097,7 @@
         <v>40000</v>
       </c>
       <c r="H237" t="n">
-        <v>0.3880494505494506</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="238">
@@ -7125,7 +7125,7 @@
         <v>40000</v>
       </c>
       <c r="H238" t="n">
-        <v>1.125343406593407</v>
+        <v>1.115384615384615</v>
       </c>
     </row>
     <row r="239">
@@ -7153,7 +7153,7 @@
         <v>40000</v>
       </c>
       <c r="H239" t="n">
-        <v>0.7928176795580111</v>
+        <v>0.7831491712707183</v>
       </c>
     </row>
     <row r="240">
@@ -7181,7 +7181,7 @@
         <v>40000</v>
       </c>
       <c r="H240" t="n">
-        <v>0.2831491712707183</v>
+        <v>0.2796961325966851</v>
       </c>
     </row>
     <row r="241">
@@ -7237,7 +7237,7 @@
         <v>40000</v>
       </c>
       <c r="H242" t="n">
-        <v>0.5321132596685083</v>
+        <v>0.524171270718232</v>
       </c>
     </row>
     <row r="243">
@@ -7293,7 +7293,7 @@
         <v>40000</v>
       </c>
       <c r="H244" t="n">
-        <v>0.5178571428571428</v>
+        <v>0.5078983516483516</v>
       </c>
     </row>
     <row r="245">
@@ -7321,7 +7321,7 @@
         <v>40000</v>
       </c>
       <c r="H245" t="n">
-        <v>0.1785714285714285</v>
+        <v>0.1751373626373626</v>
       </c>
     </row>
     <row r="246">
@@ -7349,7 +7349,7 @@
         <v>40000</v>
       </c>
       <c r="H246" t="n">
-        <v>0.2320441988950276</v>
+        <v>0.2209944751381215</v>
       </c>
     </row>
     <row r="247">
@@ -7377,7 +7377,7 @@
         <v>40000</v>
       </c>
       <c r="H247" t="n">
-        <v>0.07251381215469613</v>
+        <v>0.06906077348066299</v>
       </c>
     </row>
     <row r="248">
@@ -7405,7 +7405,7 @@
         <v>40000</v>
       </c>
       <c r="H248" t="n">
-        <v>0.4728260869565217</v>
+        <v>0.4701086956521739</v>
       </c>
     </row>
     <row r="249">
@@ -7433,7 +7433,7 @@
         <v>40000</v>
       </c>
       <c r="H249" t="n">
-        <v>1.950407608695652</v>
+        <v>1.939198369565217</v>
       </c>
     </row>
     <row r="250">
@@ -7517,7 +7517,7 @@
         <v>5000</v>
       </c>
       <c r="H252" t="n">
-        <v>2.376358695652174</v>
+        <v>2.361413043478261</v>
       </c>
     </row>
     <row r="253">
@@ -7545,7 +7545,7 @@
         <v>40000</v>
       </c>
       <c r="H253" t="n">
-        <v>1.2421875</v>
+        <v>1.234375</v>
       </c>
     </row>
     <row r="254">
@@ -7573,7 +7573,7 @@
         <v>65000</v>
       </c>
       <c r="H254" t="n">
-        <v>0.4444060773480663</v>
+        <v>0.4412983425414365</v>
       </c>
     </row>
     <row r="255">
@@ -7601,7 +7601,7 @@
         <v>65000</v>
       </c>
       <c r="H255" t="n">
-        <v>1.728245856353591</v>
+        <v>1.716160220994475</v>
       </c>
     </row>
     <row r="256">
@@ -7629,7 +7629,7 @@
         <v>40000</v>
       </c>
       <c r="H256" t="n">
-        <v>1.435782967032967</v>
+        <v>1.423076923076923</v>
       </c>
     </row>
     <row r="257">
@@ -7657,7 +7657,7 @@
         <v>40000</v>
       </c>
       <c r="H257" t="n">
-        <v>0.3880494505494506</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="258">
@@ -7685,7 +7685,7 @@
         <v>65000</v>
       </c>
       <c r="H258" t="n">
-        <v>0.3114640883977901</v>
+        <v>0.3076657458563536</v>
       </c>
     </row>
     <row r="259">
@@ -7713,7 +7713,7 @@
         <v>40000</v>
       </c>
       <c r="H259" t="n">
-        <v>1.104281767955801</v>
+        <v>1.090814917127072</v>
       </c>
     </row>
     <row r="260">
@@ -7769,7 +7769,7 @@
         <v>5000</v>
       </c>
       <c r="H261" t="n">
-        <v>0.9716850828729282</v>
+        <v>0.9571823204419889</v>
       </c>
     </row>
     <row r="262">
@@ -7797,7 +7797,7 @@
         <v>40000</v>
       </c>
       <c r="H262" t="n">
-        <v>0.5783839779005525</v>
+        <v>0.5697513812154696</v>
       </c>
     </row>
     <row r="263">
@@ -7853,7 +7853,7 @@
         <v>65000</v>
       </c>
       <c r="H264" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.2101648351648352</v>
       </c>
     </row>
     <row r="265">
@@ -7881,7 +7881,7 @@
         <v>10000</v>
       </c>
       <c r="H265" t="n">
-        <v>0.625</v>
+        <v>0.6129807692307693</v>
       </c>
     </row>
     <row r="266">
@@ -7909,7 +7909,7 @@
         <v>40000</v>
       </c>
       <c r="H266" t="n">
-        <v>0.07976519337016574</v>
+        <v>0.07596685082872928</v>
       </c>
     </row>
     <row r="267">
@@ -7937,7 +7937,7 @@
         <v>40000</v>
       </c>
       <c r="H267" t="n">
-        <v>0.2175414364640884</v>
+        <v>0.2071823204419889</v>
       </c>
     </row>
     <row r="268">
@@ -7965,7 +7965,7 @@
         <v>65000</v>
       </c>
       <c r="H268" t="n">
-        <v>1.891304347826087</v>
+        <v>1.880434782608696</v>
       </c>
     </row>
     <row r="269">
@@ -7993,7 +7993,7 @@
         <v>40000</v>
       </c>
       <c r="H269" t="n">
-        <v>0.8274456521739131</v>
+        <v>0.8226902173913043</v>
       </c>
     </row>
     <row r="270">
@@ -8021,7 +8021,7 @@
         <v>40000</v>
       </c>
       <c r="H270" t="n">
-        <v>1.134171195652174</v>
+        <v>1.127038043478261</v>
       </c>
     </row>
     <row r="271">
@@ -8105,7 +8105,7 @@
         <v>2500</v>
       </c>
       <c r="H273" t="n">
-        <v>2.268342391304348</v>
+        <v>2.254076086956522</v>
       </c>
     </row>
     <row r="274">
@@ -8133,7 +8133,7 @@
         <v>40000</v>
       </c>
       <c r="H274" t="n">
-        <v>0.7406767955801105</v>
+        <v>0.7354972375690608</v>
       </c>
     </row>
     <row r="275">
@@ -8161,7 +8161,7 @@
         <v>10000</v>
       </c>
       <c r="H275" t="n">
-        <v>1.678867403314917</v>
+        <v>1.667127071823205</v>
       </c>
     </row>
     <row r="276">
@@ -8189,7 +8189,7 @@
         <v>40000</v>
       </c>
       <c r="H276" t="n">
-        <v>1.280563186813187</v>
+        <v>1.269230769230769</v>
       </c>
     </row>
     <row r="277">
@@ -8217,7 +8217,7 @@
         <v>40000</v>
       </c>
       <c r="H277" t="n">
-        <v>0.7372939560439561</v>
+        <v>0.7307692307692307</v>
       </c>
     </row>
     <row r="278">
@@ -8245,7 +8245,7 @@
         <v>40000</v>
       </c>
       <c r="H278" t="n">
-        <v>1.047651933701657</v>
+        <v>1.034875690607735</v>
       </c>
     </row>
     <row r="279">
@@ -8273,7 +8273,7 @@
         <v>40000</v>
       </c>
       <c r="H279" t="n">
-        <v>0.6512430939226519</v>
+        <v>0.6433011049723757</v>
       </c>
     </row>
     <row r="280">
@@ -8329,7 +8329,7 @@
         <v>65000</v>
       </c>
       <c r="H281" t="n">
-        <v>0.4395718232044199</v>
+        <v>0.4330110497237569</v>
       </c>
     </row>
     <row r="282">
@@ -8357,7 +8357,7 @@
         <v>40000</v>
       </c>
       <c r="H282" t="n">
-        <v>0.6428571428571428</v>
+        <v>0.6304945054945055</v>
       </c>
     </row>
     <row r="283">
@@ -8385,7 +8385,7 @@
         <v>65000</v>
       </c>
       <c r="H283" t="n">
-        <v>0.3928571428571428</v>
+        <v>0.3853021978021978</v>
       </c>
     </row>
     <row r="284">
@@ -8413,7 +8413,7 @@
         <v>80000</v>
       </c>
       <c r="H284" t="n">
-        <v>0.2465469613259668</v>
+        <v>0.2348066298342542</v>
       </c>
     </row>
     <row r="285">
@@ -8441,7 +8441,7 @@
         <v>40000</v>
       </c>
       <c r="H285" t="n">
-        <v>0.1885359116022099</v>
+        <v>0.1795580110497238</v>
       </c>
     </row>
     <row r="286">
@@ -8469,7 +8469,7 @@
         <v>40000</v>
       </c>
       <c r="H286" t="n">
-        <v>1.24116847826087</v>
+        <v>1.234035326086957</v>
       </c>
     </row>
     <row r="287">
@@ -8497,7 +8497,7 @@
         <v>65000</v>
       </c>
       <c r="H287" t="n">
-        <v>1.891304347826087</v>
+        <v>1.880434782608696</v>
       </c>
     </row>
     <row r="288">
@@ -8525,7 +8525,7 @@
         <v>1200</v>
       </c>
       <c r="H288" t="n">
-        <v>2.646399456521739</v>
+        <v>2.629755434782609</v>
       </c>
     </row>
     <row r="289">
@@ -8609,7 +8609,7 @@
         <v>40000</v>
       </c>
       <c r="H291" t="n">
-        <v>0.7021059782608695</v>
+        <v>0.6976902173913043</v>
       </c>
     </row>
     <row r="292">
@@ -8665,7 +8665,7 @@
         <v>65000</v>
       </c>
       <c r="H293" t="n">
-        <v>1.234461325966851</v>
+        <v>1.225828729281768</v>
       </c>
     </row>
     <row r="294">
@@ -8693,7 +8693,7 @@
         <v>65000</v>
       </c>
       <c r="H294" t="n">
-        <v>1.431975138121547</v>
+        <v>1.421961325966851</v>
       </c>
     </row>
     <row r="295">
@@ -8721,7 +8721,7 @@
         <v>40000</v>
       </c>
       <c r="H295" t="n">
-        <v>1.086538461538462</v>
+        <v>1.076923076923077</v>
       </c>
     </row>
     <row r="296">
@@ -8749,7 +8749,7 @@
         <v>40000</v>
       </c>
       <c r="H296" t="n">
-        <v>1.202953296703297</v>
+        <v>1.192307692307692</v>
       </c>
     </row>
     <row r="297">
@@ -8777,7 +8777,7 @@
         <v>100000</v>
       </c>
       <c r="H297" t="n">
-        <v>0.9343922651933702</v>
+        <v>0.9229972375690608</v>
       </c>
     </row>
     <row r="298">
@@ -8805,7 +8805,7 @@
         <v>40000</v>
       </c>
       <c r="H298" t="n">
-        <v>0.9060773480662984</v>
+        <v>0.8950276243093923</v>
       </c>
     </row>
     <row r="299">
@@ -8861,7 +8861,7 @@
         <v>40000</v>
       </c>
       <c r="H300" t="n">
-        <v>0.3238950276243094</v>
+        <v>0.319060773480663</v>
       </c>
     </row>
     <row r="301">
@@ -8889,7 +8889,7 @@
         <v>100000</v>
       </c>
       <c r="H301" t="n">
-        <v>0.5892857142857143</v>
+        <v>0.5779532967032966</v>
       </c>
     </row>
     <row r="302">
@@ -8917,7 +8917,7 @@
         <v>40000</v>
       </c>
       <c r="H302" t="n">
-        <v>0.5535714285714285</v>
+        <v>0.5429258241758241</v>
       </c>
     </row>
     <row r="303">
@@ -8945,7 +8945,7 @@
         <v>65000</v>
       </c>
       <c r="H303" t="n">
-        <v>0.224792817679558</v>
+        <v>0.2140883977900553</v>
       </c>
     </row>
     <row r="304">
@@ -8973,7 +8973,7 @@
         <v>7000</v>
       </c>
       <c r="H304" t="n">
-        <v>0.2537983425414365</v>
+        <v>0.2417127071823204</v>
       </c>
     </row>
     <row r="305">
@@ -9001,7 +9001,7 @@
         <v>16000</v>
       </c>
       <c r="H305" t="n">
-        <v>1.654891304347826</v>
+        <v>1.645380434782609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>